<commit_message>
ajustes para o case tecnico
</commit_message>
<xml_diff>
--- a/automacao_fd_ld/public/Template Lista de Instrumentos.xlsx
+++ b/automacao_fd_ld/public/Template Lista de Instrumentos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae86ac8ea500c045/Documentos/GitHub/-Lista-de-Itens-para-Folha-de-dados/automacao_fd_ld/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugol\OneDrive\Área de Trabalho\folhadedados\automacao_fd_ld\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0C23160-D036-4C22-81A4-36D9CF56219F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FE5E94-CFAF-4ECE-95CF-B0D7CCA8C37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="9" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t xml:space="preserve">LISTA DE INSTRUMENTOS </t>
   </si>
@@ -128,9 +128,6 @@
       </rPr>
       <t>Area</t>
     </r>
-  </si>
-  <si>
-    <t>CENTRO DE ENGENHARIA TECHNIK</t>
   </si>
   <si>
     <r>
@@ -1442,13 +1439,220 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1457,9 +1661,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1477,210 +1678,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1704,166 +1701,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>360046</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>135254</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5155" name="Imagem 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C062E2DE-48B7-7C82-0404-FC367C1D7F97}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="4936" r="10054"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="142875" y="47625"/>
-          <a:ext cx="1360668" cy="560897"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>83344</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>137769</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1780599</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>435223</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAA953C3-C6E1-47A8-B1D7-B43AFC680AAA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="4936" t="23718" r="10054" b="20513"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="500063" y="137769"/>
-          <a:ext cx="3160091" cy="742272"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2258,8 +2095,8 @@
   </sheetPr>
   <dimension ref="A1:N432"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2272,330 +2109,328 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="125"/>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="123" t="s">
+      <c r="A1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="131" t="s">
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="133"/>
-      <c r="K1" s="133"/>
-      <c r="L1" s="133"/>
-      <c r="M1" s="133"/>
-      <c r="N1" s="134"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="76"/>
     </row>
     <row r="2" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="108"/>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="120"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="77"/>
     </row>
     <row r="3" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="108"/>
-      <c r="B3" s="109"/>
-      <c r="C3" s="109"/>
-      <c r="D3" s="87" t="s">
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="87" t="s">
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="127">
+      <c r="L3" s="69">
         <v>1</v>
       </c>
-      <c r="M3" s="129" t="s">
+      <c r="M3" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="121">
+      <c r="N3" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="111"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="114"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
-      <c r="J4" s="119"/>
-      <c r="K4" s="114"/>
-      <c r="L4" s="128"/>
-      <c r="M4" s="130"/>
-      <c r="N4" s="122"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="56"/>
     </row>
     <row r="5" spans="1:14" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="105"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="87" t="s">
+      <c r="A5" s="78"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
-      <c r="H5" s="115"/>
-      <c r="I5" s="115"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="116"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="83"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="108"/>
-      <c r="B6" s="109"/>
-      <c r="C6" s="110"/>
-      <c r="D6" s="114"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="117"/>
-      <c r="H6" s="117"/>
-      <c r="I6" s="117"/>
-      <c r="J6" s="117"/>
-      <c r="K6" s="117"/>
-      <c r="L6" s="117"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="118"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="85"/>
     </row>
     <row r="7" spans="1:14" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="108"/>
-      <c r="B7" s="109"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="87" t="s">
+      <c r="A7" s="61"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="115"/>
-      <c r="F7" s="115"/>
-      <c r="G7" s="115"/>
-      <c r="H7" s="115"/>
-      <c r="I7" s="115"/>
-      <c r="J7" s="115"/>
-      <c r="K7" s="115"/>
-      <c r="L7" s="115"/>
-      <c r="M7" s="115"/>
-      <c r="N7" s="116"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="83"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="111"/>
-      <c r="B8" s="112"/>
-      <c r="C8" s="113"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="119"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="119"/>
-      <c r="N8" s="120"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="77"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="92"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="82"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="87" t="s">
+      <c r="E9" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="99"/>
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="99"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="99"/>
+      <c r="M9" s="99"/>
+      <c r="N9" s="100"/>
+    </row>
+    <row r="10" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="95"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="101"/>
+      <c r="F10" s="101"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="101"/>
+      <c r="K10" s="101"/>
+      <c r="L10" s="101"/>
+      <c r="M10" s="101"/>
+      <c r="N10" s="102"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="89"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="89"/>
-      <c r="I9" s="89"/>
-      <c r="J9" s="89"/>
-      <c r="K9" s="89"/>
-      <c r="L9" s="89"/>
-      <c r="M9" s="89"/>
-      <c r="N9" s="90"/>
-    </row>
-    <row r="10" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="84"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="91"/>
-      <c r="I10" s="91"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="91"/>
-      <c r="L10" s="91"/>
-      <c r="M10" s="91"/>
-      <c r="N10" s="92"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="93" t="s">
+      <c r="B11" s="104"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="104"/>
+      <c r="F11" s="104"/>
+      <c r="G11" s="104"/>
+      <c r="H11" s="104"/>
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="104"/>
+      <c r="N11" s="105"/>
+    </row>
+    <row r="12" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="106"/>
+      <c r="B12" s="107"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="107"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="107"/>
+      <c r="K12" s="107"/>
+      <c r="L12" s="107"/>
+      <c r="M12" s="107"/>
+      <c r="N12" s="108"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="94"/>
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="94"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="94"/>
-      <c r="L11" s="94"/>
-      <c r="M11" s="94"/>
-      <c r="N11" s="95"/>
-    </row>
-    <row r="12" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="96"/>
-      <c r="B12" s="97"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="97"/>
-      <c r="H12" s="97"/>
-      <c r="I12" s="97"/>
-      <c r="J12" s="97"/>
-      <c r="K12" s="97"/>
-      <c r="L12" s="97"/>
-      <c r="M12" s="97"/>
-      <c r="N12" s="98"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="99" t="s">
+      <c r="B13" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="101" t="s">
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="111"/>
+      <c r="M13" s="111"/>
+      <c r="N13" s="112"/>
+    </row>
+    <row r="14" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="110"/>
+      <c r="B14" s="113"/>
+      <c r="C14" s="113"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="113"/>
+      <c r="I14" s="113"/>
+      <c r="J14" s="113"/>
+      <c r="K14" s="113"/>
+      <c r="L14" s="113"/>
+      <c r="M14" s="113"/>
+      <c r="N14" s="114"/>
+    </row>
+    <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="101"/>
-      <c r="H13" s="101"/>
-      <c r="I13" s="101"/>
-      <c r="J13" s="101"/>
-      <c r="K13" s="101"/>
-      <c r="L13" s="101"/>
-      <c r="M13" s="101"/>
-      <c r="N13" s="102"/>
-    </row>
-    <row r="14" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="100"/>
-      <c r="B14" s="103"/>
-      <c r="C14" s="103"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="103"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="103"/>
-      <c r="I14" s="103"/>
-      <c r="J14" s="103"/>
-      <c r="K14" s="103"/>
-      <c r="L14" s="103"/>
-      <c r="M14" s="103"/>
-      <c r="N14" s="104"/>
-    </row>
-    <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="76" t="s">
+      <c r="B15" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="77" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="77"/>
-      <c r="L15" s="77"/>
-      <c r="M15" s="77"/>
-      <c r="N15" s="78"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="88"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="89"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
-      <c r="B16" s="79"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="79"/>
-      <c r="N16" s="80"/>
+      <c r="A16" s="87"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="90"/>
+      <c r="L16" s="90"/>
+      <c r="M16" s="90"/>
+      <c r="N16" s="91"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="60">
+      <c r="A17" s="87">
         <v>1</v>
       </c>
-      <c r="B17" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="58"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="59"/>
+      <c r="B17" s="127" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="127"/>
+      <c r="D17" s="127"/>
+      <c r="E17" s="127"/>
+      <c r="F17" s="127"/>
+      <c r="G17" s="127"/>
+      <c r="H17" s="127"/>
+      <c r="I17" s="127"/>
+      <c r="J17" s="127"/>
+      <c r="K17" s="127"/>
+      <c r="L17" s="127"/>
+      <c r="M17" s="127"/>
+      <c r="N17" s="128"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="60"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="58"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="59"/>
+      <c r="A18" s="87"/>
+      <c r="B18" s="127"/>
+      <c r="C18" s="127"/>
+      <c r="D18" s="127"/>
+      <c r="E18" s="127"/>
+      <c r="F18" s="127"/>
+      <c r="G18" s="127"/>
+      <c r="H18" s="127"/>
+      <c r="I18" s="127"/>
+      <c r="J18" s="127"/>
+      <c r="K18" s="127"/>
+      <c r="L18" s="127"/>
+      <c r="M18" s="127"/>
+      <c r="N18" s="128"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
@@ -2742,7 +2577,7 @@
       <c r="N27" s="15"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
+      <c r="A28" s="123"/>
       <c r="B28" s="52"/>
       <c r="C28" s="52"/>
       <c r="D28" s="52"/>
@@ -2758,7 +2593,7 @@
       <c r="N28" s="15"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
+      <c r="A29" s="123"/>
       <c r="B29" s="52"/>
       <c r="C29" s="52"/>
       <c r="D29" s="52"/>
@@ -2774,7 +2609,7 @@
       <c r="N29" s="15"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
+      <c r="A30" s="123"/>
       <c r="B30" s="52"/>
       <c r="C30" s="52"/>
       <c r="D30" s="52"/>
@@ -2854,7 +2689,7 @@
       <c r="N34" s="15"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="55"/>
+      <c r="A35" s="123"/>
       <c r="B35" s="52"/>
       <c r="C35" s="52"/>
       <c r="D35" s="52"/>
@@ -2870,7 +2705,7 @@
       <c r="N35" s="15"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="55"/>
+      <c r="A36" s="123"/>
       <c r="B36" s="52"/>
       <c r="C36" s="52"/>
       <c r="D36" s="52"/>
@@ -2966,38 +2801,38 @@
       <c r="N41" s="13"/>
     </row>
     <row r="42" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="61" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="62"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="62"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="62"/>
-      <c r="J42" s="62"/>
-      <c r="K42" s="62"/>
-      <c r="L42" s="62"/>
-      <c r="M42" s="62"/>
-      <c r="N42" s="63"/>
+      <c r="A42" s="129" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="130"/>
+      <c r="C42" s="130"/>
+      <c r="D42" s="130"/>
+      <c r="E42" s="130"/>
+      <c r="F42" s="130"/>
+      <c r="G42" s="130"/>
+      <c r="H42" s="130"/>
+      <c r="I42" s="130"/>
+      <c r="J42" s="130"/>
+      <c r="K42" s="130"/>
+      <c r="L42" s="130"/>
+      <c r="M42" s="130"/>
+      <c r="N42" s="131"/>
     </row>
     <row r="43" spans="1:14" ht="13.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="64"/>
-      <c r="B43" s="65"/>
-      <c r="C43" s="65"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="65"/>
-      <c r="G43" s="65"/>
-      <c r="H43" s="65"/>
-      <c r="I43" s="65"/>
-      <c r="J43" s="65"/>
-      <c r="K43" s="65"/>
-      <c r="L43" s="65"/>
-      <c r="M43" s="65"/>
-      <c r="N43" s="66"/>
+      <c r="A43" s="132"/>
+      <c r="B43" s="133"/>
+      <c r="C43" s="133"/>
+      <c r="D43" s="133"/>
+      <c r="E43" s="133"/>
+      <c r="F43" s="133"/>
+      <c r="G43" s="133"/>
+      <c r="H43" s="133"/>
+      <c r="I43" s="133"/>
+      <c r="J43" s="133"/>
+      <c r="K43" s="133"/>
+      <c r="L43" s="133"/>
+      <c r="M43" s="133"/>
+      <c r="N43" s="134"/>
     </row>
     <row r="44" spans="1:14" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
@@ -3016,84 +2851,84 @@
       <c r="N44" s="18"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="55"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
-      <c r="N45" s="57"/>
+      <c r="A45" s="123"/>
+      <c r="B45" s="121"/>
+      <c r="C45" s="121"/>
+      <c r="D45" s="121"/>
+      <c r="E45" s="121"/>
+      <c r="F45" s="121"/>
+      <c r="G45" s="121"/>
+      <c r="H45" s="121"/>
+      <c r="I45" s="121"/>
+      <c r="J45" s="121"/>
+      <c r="K45" s="121"/>
+      <c r="L45" s="121"/>
+      <c r="M45" s="121"/>
+      <c r="N45" s="122"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="55"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="56"/>
-      <c r="L46" s="56"/>
-      <c r="M46" s="56"/>
-      <c r="N46" s="57"/>
+      <c r="A46" s="123"/>
+      <c r="B46" s="121"/>
+      <c r="C46" s="121"/>
+      <c r="D46" s="121"/>
+      <c r="E46" s="121"/>
+      <c r="F46" s="121"/>
+      <c r="G46" s="121"/>
+      <c r="H46" s="121"/>
+      <c r="I46" s="121"/>
+      <c r="J46" s="121"/>
+      <c r="K46" s="121"/>
+      <c r="L46" s="121"/>
+      <c r="M46" s="121"/>
+      <c r="N46" s="122"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="55"/>
-      <c r="B47" s="56"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
-      <c r="K47" s="56"/>
-      <c r="L47" s="56"/>
-      <c r="M47" s="56"/>
-      <c r="N47" s="57"/>
+      <c r="A47" s="123"/>
+      <c r="B47" s="121"/>
+      <c r="C47" s="121"/>
+      <c r="D47" s="121"/>
+      <c r="E47" s="121"/>
+      <c r="F47" s="121"/>
+      <c r="G47" s="121"/>
+      <c r="H47" s="121"/>
+      <c r="I47" s="121"/>
+      <c r="J47" s="121"/>
+      <c r="K47" s="121"/>
+      <c r="L47" s="121"/>
+      <c r="M47" s="121"/>
+      <c r="N47" s="122"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="55"/>
-      <c r="B48" s="56"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="56"/>
-      <c r="I48" s="56"/>
-      <c r="J48" s="56"/>
-      <c r="K48" s="56"/>
-      <c r="L48" s="56"/>
-      <c r="M48" s="56"/>
-      <c r="N48" s="57"/>
+      <c r="A48" s="123"/>
+      <c r="B48" s="121"/>
+      <c r="C48" s="121"/>
+      <c r="D48" s="121"/>
+      <c r="E48" s="121"/>
+      <c r="F48" s="121"/>
+      <c r="G48" s="121"/>
+      <c r="H48" s="121"/>
+      <c r="I48" s="121"/>
+      <c r="J48" s="121"/>
+      <c r="K48" s="121"/>
+      <c r="L48" s="121"/>
+      <c r="M48" s="121"/>
+      <c r="N48" s="122"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="55"/>
-      <c r="B49" s="56"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="56"/>
-      <c r="I49" s="56"/>
-      <c r="J49" s="56"/>
-      <c r="K49" s="56"/>
-      <c r="L49" s="56"/>
-      <c r="M49" s="56"/>
-      <c r="N49" s="57"/>
+      <c r="A49" s="123"/>
+      <c r="B49" s="121"/>
+      <c r="C49" s="121"/>
+      <c r="D49" s="121"/>
+      <c r="E49" s="121"/>
+      <c r="F49" s="121"/>
+      <c r="G49" s="121"/>
+      <c r="H49" s="121"/>
+      <c r="I49" s="121"/>
+      <c r="J49" s="121"/>
+      <c r="K49" s="121"/>
+      <c r="L49" s="121"/>
+      <c r="M49" s="121"/>
+      <c r="N49" s="122"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
@@ -3256,203 +3091,203 @@
       <c r="N59" s="10"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="55"/>
-      <c r="B60" s="56"/>
-      <c r="C60" s="56"/>
-      <c r="D60" s="56"/>
-      <c r="E60" s="56"/>
-      <c r="F60" s="56"/>
-      <c r="G60" s="56"/>
-      <c r="H60" s="56"/>
-      <c r="I60" s="56"/>
-      <c r="J60" s="56"/>
-      <c r="K60" s="56"/>
-      <c r="L60" s="56"/>
-      <c r="M60" s="56"/>
-      <c r="N60" s="57"/>
+      <c r="A60" s="123"/>
+      <c r="B60" s="121"/>
+      <c r="C60" s="121"/>
+      <c r="D60" s="121"/>
+      <c r="E60" s="121"/>
+      <c r="F60" s="121"/>
+      <c r="G60" s="121"/>
+      <c r="H60" s="121"/>
+      <c r="I60" s="121"/>
+      <c r="J60" s="121"/>
+      <c r="K60" s="121"/>
+      <c r="L60" s="121"/>
+      <c r="M60" s="121"/>
+      <c r="N60" s="122"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="55"/>
-      <c r="B61" s="56"/>
-      <c r="C61" s="56"/>
-      <c r="D61" s="56"/>
-      <c r="E61" s="56"/>
-      <c r="F61" s="56"/>
-      <c r="G61" s="56"/>
-      <c r="H61" s="56"/>
-      <c r="I61" s="56"/>
-      <c r="J61" s="56"/>
-      <c r="K61" s="56"/>
-      <c r="L61" s="56"/>
-      <c r="M61" s="56"/>
-      <c r="N61" s="57"/>
+      <c r="A61" s="123"/>
+      <c r="B61" s="121"/>
+      <c r="C61" s="121"/>
+      <c r="D61" s="121"/>
+      <c r="E61" s="121"/>
+      <c r="F61" s="121"/>
+      <c r="G61" s="121"/>
+      <c r="H61" s="121"/>
+      <c r="I61" s="121"/>
+      <c r="J61" s="121"/>
+      <c r="K61" s="121"/>
+      <c r="L61" s="121"/>
+      <c r="M61" s="121"/>
+      <c r="N61" s="122"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="9"/>
-      <c r="B62" s="56"/>
-      <c r="C62" s="56"/>
-      <c r="D62" s="56"/>
-      <c r="E62" s="56"/>
-      <c r="F62" s="56"/>
-      <c r="G62" s="56"/>
-      <c r="H62" s="56"/>
-      <c r="I62" s="56"/>
-      <c r="J62" s="56"/>
-      <c r="K62" s="56"/>
-      <c r="L62" s="56"/>
-      <c r="M62" s="56"/>
-      <c r="N62" s="57"/>
+      <c r="B62" s="121"/>
+      <c r="C62" s="121"/>
+      <c r="D62" s="121"/>
+      <c r="E62" s="121"/>
+      <c r="F62" s="121"/>
+      <c r="G62" s="121"/>
+      <c r="H62" s="121"/>
+      <c r="I62" s="121"/>
+      <c r="J62" s="121"/>
+      <c r="K62" s="121"/>
+      <c r="L62" s="121"/>
+      <c r="M62" s="121"/>
+      <c r="N62" s="122"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="55"/>
-      <c r="B63" s="56"/>
-      <c r="C63" s="56"/>
-      <c r="D63" s="56"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56"/>
-      <c r="H63" s="56"/>
-      <c r="I63" s="56"/>
-      <c r="J63" s="56"/>
-      <c r="K63" s="56"/>
-      <c r="L63" s="56"/>
-      <c r="M63" s="56"/>
-      <c r="N63" s="57"/>
+      <c r="A63" s="123"/>
+      <c r="B63" s="121"/>
+      <c r="C63" s="121"/>
+      <c r="D63" s="121"/>
+      <c r="E63" s="121"/>
+      <c r="F63" s="121"/>
+      <c r="G63" s="121"/>
+      <c r="H63" s="121"/>
+      <c r="I63" s="121"/>
+      <c r="J63" s="121"/>
+      <c r="K63" s="121"/>
+      <c r="L63" s="121"/>
+      <c r="M63" s="121"/>
+      <c r="N63" s="122"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="55"/>
-      <c r="B64" s="56"/>
-      <c r="C64" s="56"/>
-      <c r="D64" s="56"/>
-      <c r="E64" s="56"/>
-      <c r="F64" s="56"/>
-      <c r="G64" s="56"/>
-      <c r="H64" s="56"/>
-      <c r="I64" s="56"/>
-      <c r="J64" s="56"/>
-      <c r="K64" s="56"/>
-      <c r="L64" s="56"/>
-      <c r="M64" s="56"/>
-      <c r="N64" s="57"/>
+      <c r="A64" s="123"/>
+      <c r="B64" s="121"/>
+      <c r="C64" s="121"/>
+      <c r="D64" s="121"/>
+      <c r="E64" s="121"/>
+      <c r="F64" s="121"/>
+      <c r="G64" s="121"/>
+      <c r="H64" s="121"/>
+      <c r="I64" s="121"/>
+      <c r="J64" s="121"/>
+      <c r="K64" s="121"/>
+      <c r="L64" s="121"/>
+      <c r="M64" s="121"/>
+      <c r="N64" s="122"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" s="55"/>
-      <c r="B65" s="56"/>
-      <c r="C65" s="56"/>
-      <c r="D65" s="56"/>
-      <c r="E65" s="56"/>
-      <c r="F65" s="56"/>
-      <c r="G65" s="56"/>
-      <c r="H65" s="56"/>
-      <c r="I65" s="56"/>
-      <c r="J65" s="56"/>
-      <c r="K65" s="56"/>
-      <c r="L65" s="56"/>
-      <c r="M65" s="56"/>
-      <c r="N65" s="57"/>
+      <c r="A65" s="123"/>
+      <c r="B65" s="121"/>
+      <c r="C65" s="121"/>
+      <c r="D65" s="121"/>
+      <c r="E65" s="121"/>
+      <c r="F65" s="121"/>
+      <c r="G65" s="121"/>
+      <c r="H65" s="121"/>
+      <c r="I65" s="121"/>
+      <c r="J65" s="121"/>
+      <c r="K65" s="121"/>
+      <c r="L65" s="121"/>
+      <c r="M65" s="121"/>
+      <c r="N65" s="122"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="55"/>
-      <c r="B66" s="56"/>
-      <c r="C66" s="56"/>
-      <c r="D66" s="56"/>
-      <c r="E66" s="56"/>
-      <c r="F66" s="56"/>
-      <c r="G66" s="56"/>
-      <c r="H66" s="56"/>
-      <c r="I66" s="56"/>
-      <c r="J66" s="56"/>
-      <c r="K66" s="56"/>
-      <c r="L66" s="56"/>
-      <c r="M66" s="56"/>
-      <c r="N66" s="57"/>
+      <c r="A66" s="123"/>
+      <c r="B66" s="121"/>
+      <c r="C66" s="121"/>
+      <c r="D66" s="121"/>
+      <c r="E66" s="121"/>
+      <c r="F66" s="121"/>
+      <c r="G66" s="121"/>
+      <c r="H66" s="121"/>
+      <c r="I66" s="121"/>
+      <c r="J66" s="121"/>
+      <c r="K66" s="121"/>
+      <c r="L66" s="121"/>
+      <c r="M66" s="121"/>
+      <c r="N66" s="122"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="55"/>
-      <c r="B67" s="56"/>
-      <c r="C67" s="56"/>
-      <c r="D67" s="56"/>
-      <c r="E67" s="56"/>
-      <c r="F67" s="56"/>
-      <c r="G67" s="56"/>
-      <c r="H67" s="56"/>
-      <c r="I67" s="56"/>
-      <c r="J67" s="56"/>
-      <c r="K67" s="56"/>
-      <c r="L67" s="56"/>
-      <c r="M67" s="56"/>
-      <c r="N67" s="57"/>
+      <c r="A67" s="123"/>
+      <c r="B67" s="121"/>
+      <c r="C67" s="121"/>
+      <c r="D67" s="121"/>
+      <c r="E67" s="121"/>
+      <c r="F67" s="121"/>
+      <c r="G67" s="121"/>
+      <c r="H67" s="121"/>
+      <c r="I67" s="121"/>
+      <c r="J67" s="121"/>
+      <c r="K67" s="121"/>
+      <c r="L67" s="121"/>
+      <c r="M67" s="121"/>
+      <c r="N67" s="122"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="55"/>
-      <c r="B68" s="56"/>
-      <c r="C68" s="56"/>
-      <c r="D68" s="56"/>
-      <c r="E68" s="56"/>
-      <c r="F68" s="56"/>
-      <c r="G68" s="56"/>
-      <c r="H68" s="56"/>
-      <c r="I68" s="56"/>
-      <c r="J68" s="56"/>
-      <c r="K68" s="56"/>
-      <c r="L68" s="56"/>
-      <c r="M68" s="56"/>
-      <c r="N68" s="57"/>
+      <c r="A68" s="123"/>
+      <c r="B68" s="121"/>
+      <c r="C68" s="121"/>
+      <c r="D68" s="121"/>
+      <c r="E68" s="121"/>
+      <c r="F68" s="121"/>
+      <c r="G68" s="121"/>
+      <c r="H68" s="121"/>
+      <c r="I68" s="121"/>
+      <c r="J68" s="121"/>
+      <c r="K68" s="121"/>
+      <c r="L68" s="121"/>
+      <c r="M68" s="121"/>
+      <c r="N68" s="122"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="9"/>
-      <c r="B69" s="56"/>
-      <c r="C69" s="56"/>
-      <c r="D69" s="56"/>
-      <c r="E69" s="56"/>
-      <c r="F69" s="56"/>
-      <c r="G69" s="56"/>
-      <c r="H69" s="56"/>
-      <c r="I69" s="56"/>
-      <c r="J69" s="56"/>
-      <c r="K69" s="56"/>
-      <c r="L69" s="56"/>
-      <c r="M69" s="56"/>
-      <c r="N69" s="57"/>
+      <c r="B69" s="121"/>
+      <c r="C69" s="121"/>
+      <c r="D69" s="121"/>
+      <c r="E69" s="121"/>
+      <c r="F69" s="121"/>
+      <c r="G69" s="121"/>
+      <c r="H69" s="121"/>
+      <c r="I69" s="121"/>
+      <c r="J69" s="121"/>
+      <c r="K69" s="121"/>
+      <c r="L69" s="121"/>
+      <c r="M69" s="121"/>
+      <c r="N69" s="122"/>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="55"/>
-      <c r="B70" s="56"/>
-      <c r="C70" s="56"/>
-      <c r="D70" s="56"/>
-      <c r="E70" s="56"/>
-      <c r="F70" s="56"/>
-      <c r="G70" s="56"/>
-      <c r="H70" s="56"/>
-      <c r="I70" s="56"/>
-      <c r="J70" s="56"/>
-      <c r="K70" s="56"/>
-      <c r="L70" s="56"/>
-      <c r="M70" s="56"/>
-      <c r="N70" s="57"/>
+      <c r="A70" s="123"/>
+      <c r="B70" s="121"/>
+      <c r="C70" s="121"/>
+      <c r="D70" s="121"/>
+      <c r="E70" s="121"/>
+      <c r="F70" s="121"/>
+      <c r="G70" s="121"/>
+      <c r="H70" s="121"/>
+      <c r="I70" s="121"/>
+      <c r="J70" s="121"/>
+      <c r="K70" s="121"/>
+      <c r="L70" s="121"/>
+      <c r="M70" s="121"/>
+      <c r="N70" s="122"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A71" s="73"/>
-      <c r="B71" s="74"/>
-      <c r="C71" s="74"/>
-      <c r="D71" s="74"/>
-      <c r="E71" s="74"/>
-      <c r="F71" s="74"/>
-      <c r="G71" s="74"/>
-      <c r="H71" s="74"/>
-      <c r="I71" s="74"/>
-      <c r="J71" s="74"/>
-      <c r="K71" s="74"/>
-      <c r="L71" s="74"/>
-      <c r="M71" s="74"/>
-      <c r="N71" s="75"/>
+      <c r="A71" s="124"/>
+      <c r="B71" s="125"/>
+      <c r="C71" s="125"/>
+      <c r="D71" s="125"/>
+      <c r="E71" s="125"/>
+      <c r="F71" s="125"/>
+      <c r="G71" s="125"/>
+      <c r="H71" s="125"/>
+      <c r="I71" s="125"/>
+      <c r="J71" s="125"/>
+      <c r="K71" s="125"/>
+      <c r="L71" s="125"/>
+      <c r="M71" s="125"/>
+      <c r="N71" s="126"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A72" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="B72" s="68"/>
-      <c r="C72" s="69"/>
+      <c r="A72" s="115" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72" s="116"/>
+      <c r="C72" s="117"/>
       <c r="D72" s="1">
         <v>0</v>
       </c>
@@ -3488,11 +3323,11 @@
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A73" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="B73" s="68"/>
-      <c r="C73" s="69"/>
+      <c r="A73" s="115" t="s">
+        <v>15</v>
+      </c>
+      <c r="B73" s="116"/>
+      <c r="C73" s="117"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="1"/>
@@ -3506,11 +3341,11 @@
       <c r="N73" s="2"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="B74" s="68"/>
-      <c r="C74" s="69"/>
+      <c r="A74" s="115" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" s="116"/>
+      <c r="C74" s="117"/>
       <c r="D74" s="51"/>
       <c r="E74" s="51"/>
       <c r="F74" s="4"/>
@@ -3524,11 +3359,11 @@
       <c r="N74" s="5"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A75" s="67" t="s">
-        <v>18</v>
-      </c>
-      <c r="B75" s="68"/>
-      <c r="C75" s="69"/>
+      <c r="A75" s="115" t="s">
+        <v>17</v>
+      </c>
+      <c r="B75" s="116"/>
+      <c r="C75" s="117"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="4"/>
@@ -3542,11 +3377,11 @@
       <c r="N75" s="5"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A76" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="B76" s="68"/>
-      <c r="C76" s="69"/>
+      <c r="A76" s="115" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76" s="116"/>
+      <c r="C76" s="117"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="4"/>
@@ -3560,11 +3395,11 @@
       <c r="N76" s="5"/>
     </row>
     <row r="77" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="B77" s="71"/>
-      <c r="C77" s="72"/>
+      <c r="A77" s="118" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" s="119"/>
+      <c r="C77" s="120"/>
       <c r="D77" s="8"/>
       <c r="E77" s="8"/>
       <c r="F77" s="6"/>
@@ -3594,38 +3429,6 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="D1:H2"/>
-    <mergeCell ref="A1:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:N2"/>
-    <mergeCell ref="A5:C8"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:N6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:N8"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:N16"/>
-    <mergeCell ref="A9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:N10"/>
-    <mergeCell ref="A11:N12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:N14"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="B69:N69"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="B70:N71"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="A75:C75"/>
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="B67:N68"/>
     <mergeCell ref="A28:A30"/>
@@ -3642,17 +3445,48 @@
     <mergeCell ref="A42:N43"/>
     <mergeCell ref="A45:A49"/>
     <mergeCell ref="B45:N49"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="B69:N69"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="B70:N71"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:N16"/>
+    <mergeCell ref="A9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:N10"/>
+    <mergeCell ref="A11:N12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:N14"/>
+    <mergeCell ref="A5:C8"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:N6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:N8"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="D1:H2"/>
+    <mergeCell ref="A1:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:N2"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="77" orientation="portrait" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>&amp;RPágina &amp;P de &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
     <ignoredError sqref="A15" numberStoredAsText="1"/>
   </ignoredErrors>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3663,7 +3497,7 @@
   </sheetPr>
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="55" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="55" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -3693,10 +3527,10 @@
       <c r="C1" s="34"/>
       <c r="D1" s="23"/>
       <c r="E1" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -3718,7 +3552,7 @@
       <c r="C2" s="35"/>
       <c r="D2" s="26"/>
       <c r="E2" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="31"/>
       <c r="G2" s="29"/>
@@ -3741,7 +3575,7 @@
       <c r="C3" s="34"/>
       <c r="D3" s="23"/>
       <c r="E3" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="31"/>
       <c r="G3" s="29"/>
@@ -3763,7 +3597,7 @@
       <c r="C4" s="37"/>
       <c r="D4" s="38"/>
       <c r="E4" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="40"/>
       <c r="G4" s="41"/>
@@ -3782,114 +3616,114 @@
     </row>
     <row r="5" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="135" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" s="43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K5" s="43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L5" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M5" s="45"/>
       <c r="N5" s="45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O5" s="45"/>
       <c r="P5" s="43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q5" s="43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R5" s="46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S5" s="43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="136"/>
       <c r="E6" s="47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H6" s="47" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I6" s="47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J6" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="M6" s="50" t="s">
+      <c r="N6" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="N6" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="O6" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="P6" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q6" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="R6" s="50" t="s">
-        <v>24</v>
-      </c>
       <c r="S6" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3904,35 +3738,10 @@
   <headerFooter differentFirst="1">
     <oddFooter>&amp;RPágina &amp;P de &amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="09800482-4cb0-41a3-85e1-23f7b0b2224e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e4d7e4c3-b78f-4756-8feb-bf68a8958333">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010009C6D626C8523A42B259EE5D5B1F253C" ma:contentTypeVersion="18" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="eea2274a23792c3eba8bc3d2a01aaaf5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e4d7e4c3-b78f-4756-8feb-bf68a8958333" xmlns:ns3="09800482-4cb0-41a3-85e1-23f7b0b2224e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="67581f3b53955eacb98a37a3c22db38b" ns2:_="" ns3:_="">
     <xsd:import namespace="e4d7e4c3-b78f-4756-8feb-bf68a8958333"/>
@@ -4187,40 +3996,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B16F0591-B25F-4457-AE35-CA4D86DCD50E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="e4d7e4c3-b78f-4756-8feb-bf68a8958333"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="09800482-4cb0-41a3-85e1-23f7b0b2224e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9324FDB-5C52-4749-A90B-7461683D3E0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BC0AE2F-9DEE-451C-ACED-2295A6B64563}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="09800482-4cb0-41a3-85e1-23f7b0b2224e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e4d7e4c3-b78f-4756-8feb-bf68a8958333">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D50468D2-B56C-488F-B503-440AE9926764}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4237,4 +4037,37 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BC0AE2F-9DEE-451C-ACED-2295A6B64563}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9324FDB-5C52-4749-A90B-7461683D3E0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B16F0591-B25F-4457-AE35-CA4D86DCD50E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e4d7e4c3-b78f-4756-8feb-bf68a8958333"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="09800482-4cb0-41a3-85e1-23f7b0b2224e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>